<commit_message>
Revert "Merge remote-tracking branch 'origin/anhddhe170353'"
This reverts commit 8ce738c9fcff2d9b9af2753242b5f9202060554c.
</commit_message>
<xml_diff>
--- a/ismart-server/iSmart.API/wwwroot/templates/templateAddGoods.xlsx
+++ b/ismart-server/iSmart.API/wwwroot/templates/templateAddGoods.xlsx
@@ -3,11 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FULearning\Ky9\DoAnTotNghiep\iSmart\ismart-server\iSmart.API\wwwroot\templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="GoodsTemplate" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,10 +23,98 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+  <si>
+    <t>GoodsName</t>
+  </si>
+  <si>
+    <t>GoodsCode</t>
+  </si>
+  <si>
+    <t>CategoryId</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>SupplierId</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>StatusId</t>
+  </si>
+  <si>
+    <t>StockPrice</t>
+  </si>
+  <si>
+    <t>Barcode</t>
+  </si>
+  <si>
+    <t>MaxStock</t>
+  </si>
+  <si>
+    <t>MinStock</t>
+  </si>
+  <si>
+    <t>CreatedDate</t>
+  </si>
+  <si>
+    <t>WarrantyTime</t>
+  </si>
+  <si>
+    <t>Item A</t>
+  </si>
+  <si>
+    <t>Code A</t>
+  </si>
+  <si>
+    <t>Desc A</t>
+  </si>
+  <si>
+    <t>Unit A</t>
+  </si>
+  <si>
+    <t>imgA</t>
+  </si>
+  <si>
+    <t>Item B</t>
+  </si>
+  <si>
+    <t>Code B</t>
+  </si>
+  <si>
+    <t>Desc B</t>
+  </si>
+  <si>
+    <t>Unit B</t>
+  </si>
+  <si>
+    <t>imgB</t>
+  </si>
+  <si>
+    <t>Measured Unit</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -49,8 +142,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -331,12 +433,187 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" customWidth="1"/>
+    <col min="13" max="13" width="14" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1">
+        <v>100</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1">
+        <v>200</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="K2" s="1">
+        <v>12345</v>
+      </c>
+      <c r="L2" s="1">
+        <v>50</v>
+      </c>
+      <c r="M2" s="1">
+        <v>10</v>
+      </c>
+      <c r="N2" s="3">
+        <v>44562</v>
+      </c>
+      <c r="O2" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1">
+        <v>101</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1">
+        <v>201</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="1">
+        <v>2</v>
+      </c>
+      <c r="J3" s="1">
+        <v>20.5</v>
+      </c>
+      <c r="K3" s="1">
+        <v>67890</v>
+      </c>
+      <c r="L3" s="1">
+        <v>60</v>
+      </c>
+      <c r="M3" s="1">
+        <v>20</v>
+      </c>
+      <c r="N3" s="3">
+        <v>44593</v>
+      </c>
+      <c r="O3" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>